<commit_message>
Change: Theme 3 content
</commit_message>
<xml_diff>
--- a/flashcards-tema03-williankatz.xlsx
+++ b/flashcards-tema03-williankatz.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28110"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{17C2A6B0-3D2D-43D3-B646-FD1EDCC8BB32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{26E5E027-73B1-449F-B86A-C1853C29338B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="157">
   <si>
     <t>Tópico</t>
   </si>
@@ -280,6 +280,228 @@
   </si>
   <si>
     <t>Se os área dos pixels forem similares, esta área corresponde a uma região da imagem e recebe um rótulo. E se não a similaridade, esta área é dividida, geralmente, em quatro sub-regiões de áreas iguais e cada sub-região é analisada novamente segundo o critério de similaridade.</t>
+  </si>
+  <si>
+    <t>Após a Segmentação da imagem vem...</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a rotulação, que permite realizar a contagem de regiões e objetos. A cada região estabelecida, a cada bloco ou a cada componente conexo, um valor é atribuído. </t>
+  </si>
+  <si>
+    <t>Para objetos em movimento, a importancia de extrair características...</t>
+  </si>
+  <si>
+    <t>Que sejam independentes e invariantes em relação à posição. Essas características devem ser robustas a translações, rotações e deformações, já que as imagens podem ter sido capturadas em momentos diferentes.</t>
+  </si>
+  <si>
+    <t>Categorização das características diversas utilizadas no processo de reconhecimento ou identificação de objetos em imagens.</t>
+  </si>
+  <si>
+    <t>Possui dois descritores: Forma e Aspecto.</t>
+  </si>
+  <si>
+    <t>Quando falamos de Forma</t>
+  </si>
+  <si>
+    <t>Consideramos apenas o contorno dos objetos e as regiões internas</t>
+  </si>
+  <si>
+    <t>A definição da caracteristica Dimensional, em relação a Regiões.</t>
+  </si>
+  <si>
+    <t>Seria a área, perímetro, raio, compacidade etc.</t>
+  </si>
+  <si>
+    <t>A definição da caracteristica de Inercia, em relação a Regiões.</t>
+  </si>
+  <si>
+    <t>Seria o centro geométrico, orientação, retângulo envolvente etc.</t>
+  </si>
+  <si>
+    <t>A definição da caracteristica Topológica, em relação a Regiões.</t>
+  </si>
+  <si>
+    <t>Seria componentes conectados, número de vértices, número de Euler etc.</t>
+  </si>
+  <si>
+    <t>Definição de rugosidade, em relação a características de aspecto.</t>
+  </si>
+  <si>
+    <t>Expressa o acabamento de um objeto e ajuda a detectar regularidades em superfícies</t>
+  </si>
+  <si>
+    <t>Definição de textura, em relação a características de aspecto.</t>
+  </si>
+  <si>
+    <t>Pode ser utilizada para caracterizar regularidades como sulcos ou estrias, além disso fornece padronagens de determinados tipos de material, como madeiras, rochas, tecidos etc.</t>
+  </si>
+  <si>
+    <t>Definição da Análise de Componentes Principais (ACP).</t>
+  </si>
+  <si>
+    <t>Transforma variáveis discretas em coeficientes descorrelacionados, o que permite identificar as relações entre as caraterísticas extraídas de dados.</t>
+  </si>
+  <si>
+    <t>Objetivo da Análise de Componentes Principais (ACP).</t>
+  </si>
+  <si>
+    <t>Este método tem por objetivo analisar o conjunto de características usado, visando reduzi-lo, a fim de eliminar a redundância.</t>
+  </si>
+  <si>
+    <t>Definição de processo autônomo , em relação a classificação de uma imagem.</t>
+  </si>
+  <si>
+    <t>É um processo de classificação automático, porém em um primeiro momento é necessário regular manualmente para classificação. necessitando de um humano para fornecer pré-definições possíveis.</t>
+  </si>
+  <si>
+    <t>Diferença entre a classificação supervisionada e não supervisionada.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A classificação não supervisionada agrupa dados sem exemplos prévios, enquanto a classificação supervisionada usa referências conhecidas para classificar novos dados. </t>
+  </si>
+  <si>
+    <t>Objetivo da Definição de classes, para um sistema de classificação em sua primeira etapa.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Realiza a definição de que tipo de característica o problema trata, qual é a melhor maneira, a priori, de representar esta característica, ou seja, o problema é explicitado. </t>
+  </si>
+  <si>
+    <t>Objetivo da Análise das amostras de dados, para um sistema de classificação em sua segunda etapa.</t>
+  </si>
+  <si>
+    <t>Busca identificar variáveis que permitem a discriminação do exemplo dado.</t>
+  </si>
+  <si>
+    <t>Objetivo da Definição do espaço de características, para um sistema de classificação em sua terceira etapa.</t>
+  </si>
+  <si>
+    <t>Seleciona variáveis apropriadas e forma vetores de características para os dados.</t>
+  </si>
+  <si>
+    <t>Objetivo da Construção do classificador, para um sistema de classificação em sua quarta etapa.</t>
+  </si>
+  <si>
+    <t>Define superfícies de decisão no espaço de características e constrói o classificador que usa dados de treinamento.</t>
+  </si>
+  <si>
+    <t>Objetivo da Testagem do classificador, para um sistema de classificação em sua quinta etapa.</t>
+  </si>
+  <si>
+    <t>Busca encontrar novas amostras e classificá-las.</t>
+  </si>
+  <si>
+    <t>Objetivo da Validação, para um sistema de classificação em sua sexta etapa.</t>
+  </si>
+  <si>
+    <t>Pretende verificar se o desempenho da classificação foi suficientemente bom. Caso não seja satisfatório o resultado, retorna a etapa de definição das classes.</t>
+  </si>
+  <si>
+    <t>Definição dos Métodos de reconhecimento por decisão teórica, segundo os métodos de reconhecimento de imagem. (Gonzalez e Woods (2000)).</t>
+  </si>
+  <si>
+    <t>Como primeiro método, ele faz referência à representação dos padrões na forma de vetor, seguido da busca por abordagens para agrupamento e para atribuição dos vetores de padrões a classes de padrões.</t>
+  </si>
+  <si>
+    <t>Definição dos Métodos estruturais para o reconhecimento, segundo os métodos de reconhecimento de imagem. (Gonzalez e Woods (2000)).</t>
+  </si>
+  <si>
+    <t>Como segundo método, fazem reconhecimentos estruturais, buscando apresentar os padrões de uma representação simbólica, baseiam-se em casamento de cadeias ou em modelos que tratam os padrões simbólicos como estruturas de uma linguagem artificial.</t>
+  </si>
+  <si>
+    <t>Definição dos Métodos para a interpretação de imagens, segundo os métodos de reconhecimento de imagem. (Gonzalez e Woods (2000)).</t>
+  </si>
+  <si>
+    <t>Como terceiro método, interpreta imagens, de modo a realizar uma atribuição de significado ao conjunto de elementos de imagens reconhecidas.</t>
+  </si>
+  <si>
+    <t>Existem dois métodos em particular que calculam e determinam vetores que representarão o padrão ou as classes de padrões de decisão.</t>
+  </si>
+  <si>
+    <t>Esse trabalho são feitos por classificadores,  que pode considerar a praticidade de implementação, como os classificadores pautados em distâncias; ou considerar algum elemento estatístico, que toma por base a utilização de amostras de padrões para estimar determinados parâmetros estatísticos de cada classe de padrões.</t>
+  </si>
+  <si>
+    <t>Definição dos Métodos estruturais.</t>
+  </si>
+  <si>
+    <t>Procuram realizar reconhecimento de padrão realizando relações estruturais inerentes à forma do padrão.</t>
+  </si>
+  <si>
+    <t>Definição de Casamento de números de formas, em relação a Métodos Estruturais</t>
+  </si>
+  <si>
+    <t>Refere-se à correspondência entre padrões geométricos (formas) extraídos de uma imagem e um conjunto de primitivas de padrões previamente definido.</t>
+  </si>
+  <si>
+    <t>Definição de Casamento de cadeias, em relação a Métodos Estruturais.</t>
+  </si>
+  <si>
+    <t>Envolve encontrar correspondências entre padrões (ou cadeias de caracteres) em uma imagem e um modelo previamente definido.</t>
+  </si>
+  <si>
+    <t>Definição de Métodos Sintáticos, em relação a Métodos Estruturais.</t>
+  </si>
+  <si>
+    <t>Visam ao reconhecimento sintático de padrões que estão no conjunto de primitivas de padrões que, de modo geral, são um conjunto de regras que governa suas interconexões, e um reconhecedor cuja estrutura é determinada pelo conjunto de regras da gramática.</t>
+  </si>
+  <si>
+    <t>Definição de Limitação da generalidade do problema, uma das técnicas que podem ser aplicadas na interpretação de uma imagem.</t>
+  </si>
+  <si>
+    <t>Se refere ao fato de que, embora tenhamos ferramentas automatizadas para analisar características visuais em imagens, a interpretação crítica ainda depende da percepção humana.</t>
+  </si>
+  <si>
+    <t>Definição de Grafos, uma das técnicas que podem ser aplicadas na interpretação de uma imagem.</t>
+  </si>
+  <si>
+    <t>Podem ser usados para encontrar padrões, relacionar objetos ou descobrir caminhos relevantes. Por exemplo, se quisermos identificar objetos em uma foto, podemos criar um grafo onde cada objeto é um vértice e as conexões representam relações entre eles.</t>
+  </si>
+  <si>
+    <t>Definição de Incorporação de conhecimento humano, uma das técnicas que podem ser aplicadas na interpretação de uma imagem.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Refere-se a como os seres humanos contribuem com seu entendimento e expertise para melhorar a análise e compreensão de imagens. </t>
+  </si>
+  <si>
+    <t>Definição de Sistemas de produções, uma das técnicas que podem ser aplicadas na interpretação de uma imagem.</t>
+  </si>
+  <si>
+    <t>Seria uma linha de montagem para entender e analisar visualmente o que vemos. Eles nos ajudam a “fabricar” significados a partir das imagens que encontramos. Comumente chamada de sistemas baseados em regras.</t>
+  </si>
+  <si>
+    <t>Definição de Padrão. (Gonzalez e Woods (2000))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">É uma descrição quantitativa ou estrutural de um objeto ou alguma outra entidade de interesse em uma imagem. </t>
+  </si>
+  <si>
+    <t>Definição de Classe de Padrões</t>
+  </si>
+  <si>
+    <t>É um conjunto, uma família de padrões que possui algumas propriedades em comum.</t>
+  </si>
+  <si>
+    <t>Um exemplo de relações estruturais é a estrutura em escada.</t>
+  </si>
+  <si>
+    <t>É uma estrutura que visa explorar as relações entre suas regiões.</t>
+  </si>
+  <si>
+    <t>Em relação a descrição de objetos em imagens, as caracteristicas de Representações por Cadeias são:</t>
+  </si>
+  <si>
+    <t>Usam conexões simples entre primitivas (partes) dos objetos. Essas conexões geralmente estão relacionadas à borda externa da forma.</t>
+  </si>
+  <si>
+    <t>Em relação a descrição de objetos em imagens, as caracteristicas de Descrição por Árvores são:</t>
+  </si>
+  <si>
+    <t>É mais robusta e detalhada e funciona bem para objetos organizados hierarquicamente (como partes de um todo).</t>
+  </si>
+  <si>
+    <t>Definição de Redes Neurais</t>
+  </si>
+  <si>
+    <t>São caracterizadas pelo desenvolvimento adaptativo dos coeficientes das funções de decisão através de apresentações sucessivas de conjuntos de padrões de treinamento.</t>
   </si>
 </sst>
 </file>
@@ -685,16 +907,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B42"/>
+  <dimension ref="A1:B79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="A80" sqref="A80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="65.85546875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="84.7109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="94.85546875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1">
@@ -705,7 +927,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="43.5">
+    <row r="2" spans="1:2" ht="29.25">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -713,7 +935,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="43.5">
+    <row r="3" spans="1:2" ht="29.25">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -721,7 +943,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="43.5">
+    <row r="4" spans="1:2" ht="29.25">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -729,7 +951,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="43.5">
+    <row r="5" spans="1:2" ht="29.25">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
@@ -737,7 +959,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="57.75">
+    <row r="6" spans="1:2" ht="43.5">
       <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
@@ -745,7 +967,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="43.5">
+    <row r="7" spans="1:2" ht="29.25">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
@@ -753,7 +975,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="29.25">
+    <row r="8" spans="1:2">
       <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
@@ -761,7 +983,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="57.75">
+    <row r="9" spans="1:2" ht="43.5">
       <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
@@ -769,7 +991,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="29.25">
+    <row r="10" spans="1:2">
       <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
@@ -777,7 +999,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="43.5">
+    <row r="11" spans="1:2" ht="29.25">
       <c r="A11" s="5" t="s">
         <v>20</v>
       </c>
@@ -785,7 +1007,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="87">
+    <row r="12" spans="1:2" ht="57.75">
       <c r="A12" s="3" t="s">
         <v>22</v>
       </c>
@@ -793,7 +1015,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="57.75">
+    <row r="13" spans="1:2" ht="43.5">
       <c r="A13" s="3" t="s">
         <v>24</v>
       </c>
@@ -801,7 +1023,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="43.5">
+    <row r="14" spans="1:2" ht="29.25">
       <c r="A14" s="3" t="s">
         <v>26</v>
       </c>
@@ -809,7 +1031,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="101.25">
+    <row r="15" spans="1:2" ht="72.75">
       <c r="A15" s="3" t="s">
         <v>28</v>
       </c>
@@ -825,7 +1047,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="72.75">
+    <row r="17" spans="1:2" ht="57.75">
       <c r="A17" s="3" t="s">
         <v>32</v>
       </c>
@@ -833,7 +1055,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="57.75">
+    <row r="18" spans="1:2" ht="43.5">
       <c r="A18" s="3" t="s">
         <v>34</v>
       </c>
@@ -865,7 +1087,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="57.75">
+    <row r="22" spans="1:2" ht="43.5">
       <c r="A22" s="3" t="s">
         <v>42</v>
       </c>
@@ -881,7 +1103,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="43.5">
+    <row r="24" spans="1:2" ht="29.25">
       <c r="A24" s="3" t="s">
         <v>46</v>
       </c>
@@ -897,7 +1119,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="29.25">
+    <row r="26" spans="1:2">
       <c r="A26" s="3" t="s">
         <v>50</v>
       </c>
@@ -926,7 +1148,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="43.5">
+    <row r="30" spans="1:2" ht="29.25">
       <c r="A30" s="3" t="s">
         <v>57</v>
       </c>
@@ -934,7 +1156,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="72.75">
+    <row r="31" spans="1:2" ht="43.5">
       <c r="A31" s="3" t="s">
         <v>59</v>
       </c>
@@ -942,7 +1164,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="72.75">
+    <row r="32" spans="1:2" ht="57.75">
       <c r="A32" s="3" t="s">
         <v>61</v>
       </c>
@@ -950,7 +1172,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="72.75">
+    <row r="33" spans="1:2" ht="57.75">
       <c r="A33" s="3" t="s">
         <v>63</v>
       </c>
@@ -982,7 +1204,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="57.75">
+    <row r="37" spans="1:2" ht="43.5">
       <c r="A37" s="3" t="s">
         <v>71</v>
       </c>
@@ -998,7 +1220,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="43.5">
+    <row r="39" spans="1:2" ht="29.25">
       <c r="A39" s="3" t="s">
         <v>75</v>
       </c>
@@ -1022,12 +1244,308 @@
         <v>80</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="57.75">
+    <row r="42" spans="1:2" ht="43.5">
       <c r="A42" s="3" t="s">
         <v>81</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>82</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="29.25">
+      <c r="A43" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="43.5">
+      <c r="A44" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="29.25">
+      <c r="A45" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="29.25">
+      <c r="A51" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="29.25">
+      <c r="A52" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="29.25">
+      <c r="A53" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="29.25">
+      <c r="A54" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="29.25">
+      <c r="A55" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="29.25">
+      <c r="A56" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="29.25">
+      <c r="A57" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="29.25">
+      <c r="A58" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="29.25">
+      <c r="A59" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="29.25">
+      <c r="A60" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="29.25">
+      <c r="A61" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="29.25">
+      <c r="A62" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="43.5">
+      <c r="A63" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="29.25">
+      <c r="A64" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="57.75">
+      <c r="A65" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="29.25">
+      <c r="A66" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="29.25">
+      <c r="A67" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="29.25">
+      <c r="A68" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="43.5">
+      <c r="A69" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="29.25">
+      <c r="A70" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="43.5">
+      <c r="A71" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="29.25">
+      <c r="A72" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="29.25">
+      <c r="A73" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="29.25">
+      <c r="A74" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="29.25">
+      <c r="A77" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" ht="29.25">
+      <c r="A78" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" ht="29.25">
+      <c r="A79" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>